<commit_message>
Add test data and chart
</commit_message>
<xml_diff>
--- a/ajou-assignment_seat-assignment_2021-11-01_2021-12-31.xlsx
+++ b/ajou-assignment_seat-assignment_2021-11-01_2021-12-31.xlsx
@@ -7,15 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="developer" sheetId="1" r:id="rId1"/>
-    <sheet name="raw_data" sheetId="2" r:id="rId2"/>
+    <sheet name="charts" sheetId="1" r:id="rId1"/>
+    <sheet name="developer" sheetId="2" r:id="rId2"/>
+    <sheet name="branch_cm" sheetId="3" r:id="rId3"/>
+    <sheet name="branch_aoc" sheetId="4" r:id="rId4"/>
+    <sheet name="raw_data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="127">
   <si>
     <t>main</t>
   </si>
@@ -38,6 +41,9 @@
     <t>이경민</t>
   </si>
   <si>
+    <t>weeknum</t>
+  </si>
+  <si>
     <t>sha</t>
   </si>
   <si>
@@ -48,9 +54,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>weeknum</t>
   </si>
   <si>
     <t>email</t>
@@ -466,6 +469,167 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>test</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'branch_cm'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'branch_cm'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -753,9 +917,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -819,7 +996,129 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>16831</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>44389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>-42552</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>22818</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L56"/>
   <sheetViews>
@@ -829,19 +1128,19 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>

</xml_diff>